<commit_message>
Working PLC test console with ping, add device, delete device and list device.
</commit_message>
<xml_diff>
--- a/consumption (version 1).xlsb.xlsx
+++ b/consumption (version 1).xlsb.xlsx
@@ -9,13 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8772" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PLC 1" sheetId="1" r:id="rId1"/>
+    <sheet name="Tabelle1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="17">
   <si>
     <t>send</t>
   </si>
@@ -150,12 +150,200 @@
       <t xml:space="preserve"> [V]</t>
     </r>
   </si>
+  <si>
+    <t>PLC</t>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mA]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mA]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mW]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mW]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>wake</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [V]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>V</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sleep</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [V]</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>P</t>
+    </r>
+    <r>
+      <rPr>
+        <vertAlign val="subscript"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>dif</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> [mW]</t>
+    </r>
+  </si>
+  <si>
+    <t>Mini Control cut out</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -180,8 +368,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <vertAlign val="subscript"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="48"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -200,6 +403,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9999"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -213,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -233,12 +442,32 @@
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF9999"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -2825,7 +3054,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
@@ -3213,4 +3442,1045 @@
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
   <drawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54EF9737-EC01-4798-97D4-F1573FFECD07}">
+  <dimension ref="A1:J41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K13" sqref="K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="16384" width="11.5546875" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="9">
+        <v>2</v>
+      </c>
+      <c r="B2" s="10">
+        <v>9.67</v>
+      </c>
+      <c r="C2" s="10">
+        <v>103.1</v>
+      </c>
+      <c r="D2" s="10">
+        <v>10</v>
+      </c>
+      <c r="E2" s="10">
+        <v>51.6</v>
+      </c>
+      <c r="F2" s="10">
+        <f>B2*C2</f>
+        <v>996.97699999999998</v>
+      </c>
+      <c r="G2" s="10">
+        <f>D2*E2</f>
+        <v>516</v>
+      </c>
+      <c r="H2" s="10">
+        <f>F2-G2</f>
+        <v>480.97699999999998</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="9"/>
+      <c r="B3" s="10">
+        <v>9.16</v>
+      </c>
+      <c r="C3" s="10">
+        <v>103.1</v>
+      </c>
+      <c r="D3" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="E3" s="10">
+        <v>51.5</v>
+      </c>
+      <c r="F3" s="10">
+        <f t="shared" ref="F3:F13" si="0">B3*C3</f>
+        <v>944.39599999999996</v>
+      </c>
+      <c r="G3" s="10">
+        <f t="shared" ref="G3:G13" si="1">D3*E3</f>
+        <v>489.25</v>
+      </c>
+      <c r="H3" s="10">
+        <f t="shared" ref="H3:H13" si="2">F3-G3</f>
+        <v>455.14599999999996</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="9"/>
+      <c r="B4" s="10">
+        <v>8.69</v>
+      </c>
+      <c r="C4" s="10">
+        <v>103</v>
+      </c>
+      <c r="D4" s="10">
+        <v>9</v>
+      </c>
+      <c r="E4" s="10">
+        <v>51.5</v>
+      </c>
+      <c r="F4" s="10">
+        <f t="shared" si="0"/>
+        <v>895.06999999999994</v>
+      </c>
+      <c r="G4" s="10">
+        <f t="shared" si="1"/>
+        <v>463.5</v>
+      </c>
+      <c r="H4" s="10">
+        <f t="shared" si="2"/>
+        <v>431.56999999999994</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="9"/>
+      <c r="B5" s="10">
+        <v>8.1300000000000008</v>
+      </c>
+      <c r="C5" s="10">
+        <v>100.7</v>
+      </c>
+      <c r="D5" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="E5" s="10">
+        <v>51.5</v>
+      </c>
+      <c r="F5" s="10">
+        <f t="shared" si="0"/>
+        <v>818.69100000000014</v>
+      </c>
+      <c r="G5" s="10">
+        <f t="shared" si="1"/>
+        <v>437.75</v>
+      </c>
+      <c r="H5" s="10">
+        <f t="shared" si="2"/>
+        <v>380.94100000000014</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="9"/>
+      <c r="B6" s="10">
+        <v>7.69</v>
+      </c>
+      <c r="C6" s="10">
+        <v>93.8</v>
+      </c>
+      <c r="D6" s="10">
+        <v>8</v>
+      </c>
+      <c r="E6" s="10">
+        <v>51.4</v>
+      </c>
+      <c r="F6" s="10">
+        <f t="shared" si="0"/>
+        <v>721.322</v>
+      </c>
+      <c r="G6" s="10">
+        <f t="shared" si="1"/>
+        <v>411.2</v>
+      </c>
+      <c r="H6" s="10">
+        <f t="shared" si="2"/>
+        <v>310.12200000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="9"/>
+      <c r="B7" s="10">
+        <v>7.3</v>
+      </c>
+      <c r="C7" s="10">
+        <v>87.4</v>
+      </c>
+      <c r="D7" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="E7" s="10">
+        <v>51.5</v>
+      </c>
+      <c r="F7" s="10">
+        <f t="shared" si="0"/>
+        <v>638.02</v>
+      </c>
+      <c r="G7" s="10">
+        <f t="shared" si="1"/>
+        <v>386.25</v>
+      </c>
+      <c r="H7" s="10">
+        <f t="shared" si="2"/>
+        <v>251.76999999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10">
+        <v>6.84</v>
+      </c>
+      <c r="C8" s="10">
+        <v>79.8</v>
+      </c>
+      <c r="D8" s="10">
+        <v>7</v>
+      </c>
+      <c r="E8" s="10">
+        <v>51.5</v>
+      </c>
+      <c r="F8" s="10">
+        <f t="shared" si="0"/>
+        <v>545.83199999999999</v>
+      </c>
+      <c r="G8" s="10">
+        <f t="shared" si="1"/>
+        <v>360.5</v>
+      </c>
+      <c r="H8" s="10">
+        <f t="shared" si="2"/>
+        <v>185.33199999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="9"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G9" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H9" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I9" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="J9" s="8"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11">
+        <v>6</v>
+      </c>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G10" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H10" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I10" s="8"/>
+      <c r="J10" s="8"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="11"/>
+      <c r="C11" s="11"/>
+      <c r="D11" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="E11" s="11"/>
+      <c r="F11" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G11" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H11" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I11" s="8"/>
+      <c r="J11" s="8"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11">
+        <v>5</v>
+      </c>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G12" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H12" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="8"/>
+      <c r="J12" s="8"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="G13" s="11">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="H13" s="11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I13" s="8"/>
+      <c r="J13" s="8"/>
+    </row>
+    <row r="15" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D15" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H15" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" s="9">
+        <v>1</v>
+      </c>
+      <c r="B16" s="10">
+        <v>9.64</v>
+      </c>
+      <c r="C16" s="10">
+        <v>103.5</v>
+      </c>
+      <c r="D16" s="10">
+        <v>10</v>
+      </c>
+      <c r="E16" s="10">
+        <v>52.2</v>
+      </c>
+      <c r="F16" s="10">
+        <f>B16*C16</f>
+        <v>997.74</v>
+      </c>
+      <c r="G16" s="10">
+        <f>D16*E16</f>
+        <v>522</v>
+      </c>
+      <c r="H16" s="10">
+        <f>F16-G16</f>
+        <v>475.74</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" s="9"/>
+      <c r="B17" s="10">
+        <v>9.16</v>
+      </c>
+      <c r="C17" s="10">
+        <v>103.6</v>
+      </c>
+      <c r="D17" s="10">
+        <v>9.5</v>
+      </c>
+      <c r="E17" s="10">
+        <v>52.2</v>
+      </c>
+      <c r="F17" s="10">
+        <f t="shared" ref="F17:F27" si="3">B17*C17</f>
+        <v>948.976</v>
+      </c>
+      <c r="G17" s="10">
+        <f t="shared" ref="G17:G27" si="4">D17*E17</f>
+        <v>495.90000000000003</v>
+      </c>
+      <c r="H17" s="10">
+        <f t="shared" ref="H17:H27" si="5">F17-G17</f>
+        <v>453.07599999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="10">
+        <v>8.67</v>
+      </c>
+      <c r="C18" s="10">
+        <v>103.6</v>
+      </c>
+      <c r="D18" s="10">
+        <v>9</v>
+      </c>
+      <c r="E18" s="10">
+        <v>52.2</v>
+      </c>
+      <c r="F18" s="10">
+        <f t="shared" si="3"/>
+        <v>898.21199999999999</v>
+      </c>
+      <c r="G18" s="10">
+        <f t="shared" si="4"/>
+        <v>469.8</v>
+      </c>
+      <c r="H18" s="10">
+        <f t="shared" si="5"/>
+        <v>428.41199999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="10">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="C19" s="10">
+        <v>101.4</v>
+      </c>
+      <c r="D19" s="10">
+        <v>8.5</v>
+      </c>
+      <c r="E19" s="10">
+        <v>52.1</v>
+      </c>
+      <c r="F19" s="10">
+        <f t="shared" si="3"/>
+        <v>831.48</v>
+      </c>
+      <c r="G19" s="10">
+        <f t="shared" si="4"/>
+        <v>442.85</v>
+      </c>
+      <c r="H19" s="10">
+        <f t="shared" si="5"/>
+        <v>388.63</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" s="9"/>
+      <c r="B20" s="10">
+        <v>7.65</v>
+      </c>
+      <c r="C20" s="10">
+        <v>92.8</v>
+      </c>
+      <c r="D20" s="10">
+        <v>8</v>
+      </c>
+      <c r="E20" s="10">
+        <v>52.2</v>
+      </c>
+      <c r="F20" s="10">
+        <f t="shared" si="3"/>
+        <v>709.92</v>
+      </c>
+      <c r="G20" s="10">
+        <f t="shared" si="4"/>
+        <v>417.6</v>
+      </c>
+      <c r="H20" s="10">
+        <f t="shared" si="5"/>
+        <v>292.31999999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="10">
+        <v>7.24</v>
+      </c>
+      <c r="C21" s="10">
+        <v>86.1</v>
+      </c>
+      <c r="D21" s="10">
+        <v>7.5</v>
+      </c>
+      <c r="E21" s="10">
+        <v>52.1</v>
+      </c>
+      <c r="F21" s="10">
+        <f t="shared" si="3"/>
+        <v>623.36400000000003</v>
+      </c>
+      <c r="G21" s="10">
+        <f t="shared" si="4"/>
+        <v>390.75</v>
+      </c>
+      <c r="H21" s="10">
+        <f t="shared" si="5"/>
+        <v>232.61400000000003</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="10">
+        <v>6.8</v>
+      </c>
+      <c r="C22" s="10">
+        <v>78.900000000000006</v>
+      </c>
+      <c r="D22" s="10">
+        <v>7</v>
+      </c>
+      <c r="E22" s="10">
+        <v>52.1</v>
+      </c>
+      <c r="F22" s="10">
+        <f t="shared" si="3"/>
+        <v>536.52</v>
+      </c>
+      <c r="G22" s="10">
+        <f t="shared" si="4"/>
+        <v>364.7</v>
+      </c>
+      <c r="H22" s="10">
+        <f t="shared" si="5"/>
+        <v>171.82</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="B23" s="11">
+        <v>6.37</v>
+      </c>
+      <c r="C23" s="11">
+        <v>58.6</v>
+      </c>
+      <c r="D23" s="11">
+        <v>6.5</v>
+      </c>
+      <c r="E23" s="11"/>
+      <c r="F23" s="11">
+        <f t="shared" si="3"/>
+        <v>373.28200000000004</v>
+      </c>
+      <c r="G23" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H23" s="11">
+        <f t="shared" si="5"/>
+        <v>373.28200000000004</v>
+      </c>
+      <c r="I23" s="8" t="str">
+        <f>I9</f>
+        <v>Mini Control cut out</v>
+      </c>
+      <c r="J23" s="8"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="11"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="11">
+        <v>6</v>
+      </c>
+      <c r="E24" s="11"/>
+      <c r="F24" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G24" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H24" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I24" s="8"/>
+      <c r="J24" s="8"/>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="11"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="11">
+        <v>5.5</v>
+      </c>
+      <c r="E25" s="11"/>
+      <c r="F25" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G25" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H25" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="B26" s="11"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="11">
+        <v>5</v>
+      </c>
+      <c r="E26" s="11"/>
+      <c r="F26" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G26" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H26" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I26" s="8"/>
+      <c r="J26" s="8"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="11"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="11">
+        <v>4.5</v>
+      </c>
+      <c r="E27" s="11"/>
+      <c r="F27" s="11">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+      <c r="G27" s="11">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H27" s="11">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="I27" s="8"/>
+      <c r="J27" s="8"/>
+    </row>
+    <row r="29" spans="1:10" ht="15.6" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D29" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="F29" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="9">
+        <v>4</v>
+      </c>
+      <c r="B30" s="1">
+        <v>9.6999999999999993</v>
+      </c>
+      <c r="C30" s="1">
+        <v>105</v>
+      </c>
+      <c r="D30" s="1">
+        <v>10</v>
+      </c>
+      <c r="E30" s="1">
+        <v>54</v>
+      </c>
+      <c r="F30" s="10">
+        <f>B30*C30</f>
+        <v>1018.4999999999999</v>
+      </c>
+      <c r="G30" s="10">
+        <f>D30*E30</f>
+        <v>540</v>
+      </c>
+      <c r="H30" s="10">
+        <f>F30-G30</f>
+        <v>478.49999999999989</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="1">
+        <v>9.19</v>
+      </c>
+      <c r="C31" s="1">
+        <v>105.2</v>
+      </c>
+      <c r="D31" s="1">
+        <v>9.5</v>
+      </c>
+      <c r="E31" s="1">
+        <v>52.8</v>
+      </c>
+      <c r="F31" s="10">
+        <f t="shared" ref="F31:F41" si="6">B31*C31</f>
+        <v>966.78800000000001</v>
+      </c>
+      <c r="G31" s="10">
+        <f t="shared" ref="G31:G41" si="7">D31*E31</f>
+        <v>501.59999999999997</v>
+      </c>
+      <c r="H31" s="10">
+        <f t="shared" ref="H31:H41" si="8">F31-G31</f>
+        <v>465.18800000000005</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="1">
+        <v>8.67</v>
+      </c>
+      <c r="C32" s="1">
+        <v>105.5</v>
+      </c>
+      <c r="D32" s="1">
+        <v>9</v>
+      </c>
+      <c r="E32" s="1">
+        <v>52.35</v>
+      </c>
+      <c r="F32" s="10">
+        <f t="shared" si="6"/>
+        <v>914.68499999999995</v>
+      </c>
+      <c r="G32" s="10">
+        <f t="shared" si="7"/>
+        <v>471.15000000000003</v>
+      </c>
+      <c r="H32" s="10">
+        <f t="shared" si="8"/>
+        <v>443.53499999999991</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="9"/>
+      <c r="B33" s="1">
+        <v>8.17</v>
+      </c>
+      <c r="C33" s="1">
+        <v>102.6</v>
+      </c>
+      <c r="D33" s="1">
+        <v>8.5</v>
+      </c>
+      <c r="E33" s="1">
+        <v>51.8</v>
+      </c>
+      <c r="F33" s="10">
+        <f t="shared" si="6"/>
+        <v>838.24199999999996</v>
+      </c>
+      <c r="G33" s="10">
+        <f t="shared" si="7"/>
+        <v>440.29999999999995</v>
+      </c>
+      <c r="H33" s="10">
+        <f t="shared" si="8"/>
+        <v>397.94200000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="B34" s="1">
+        <v>7.73</v>
+      </c>
+      <c r="C34" s="1">
+        <v>95.2</v>
+      </c>
+      <c r="D34" s="1">
+        <v>8</v>
+      </c>
+      <c r="E34" s="1">
+        <v>54</v>
+      </c>
+      <c r="F34" s="10">
+        <f t="shared" si="6"/>
+        <v>735.89600000000007</v>
+      </c>
+      <c r="G34" s="10">
+        <f t="shared" si="7"/>
+        <v>432</v>
+      </c>
+      <c r="H34" s="10">
+        <f t="shared" si="8"/>
+        <v>303.89600000000007</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="1">
+        <v>7.26</v>
+      </c>
+      <c r="C35" s="1">
+        <v>87.2</v>
+      </c>
+      <c r="D35" s="1">
+        <v>7.5</v>
+      </c>
+      <c r="E35" s="1">
+        <v>51.9</v>
+      </c>
+      <c r="F35" s="10">
+        <f t="shared" si="6"/>
+        <v>633.072</v>
+      </c>
+      <c r="G35" s="10">
+        <f t="shared" si="7"/>
+        <v>389.25</v>
+      </c>
+      <c r="H35" s="10">
+        <f t="shared" si="8"/>
+        <v>243.822</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="1">
+        <v>6.79</v>
+      </c>
+      <c r="C36" s="1">
+        <v>79.599999999999994</v>
+      </c>
+      <c r="D36" s="1">
+        <v>7</v>
+      </c>
+      <c r="E36" s="1">
+        <v>51.9</v>
+      </c>
+      <c r="F36" s="10">
+        <f t="shared" si="6"/>
+        <v>540.48399999999992</v>
+      </c>
+      <c r="G36" s="10">
+        <f t="shared" si="7"/>
+        <v>363.3</v>
+      </c>
+      <c r="H36" s="10">
+        <f t="shared" si="8"/>
+        <v>177.18399999999991</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" s="9"/>
+      <c r="B37" s="7">
+        <v>6.41</v>
+      </c>
+      <c r="C37" s="7">
+        <v>59.7</v>
+      </c>
+      <c r="D37" s="7">
+        <v>6.5</v>
+      </c>
+      <c r="E37" s="7">
+        <v>51.7</v>
+      </c>
+      <c r="F37" s="11">
+        <f t="shared" si="6"/>
+        <v>382.67700000000002</v>
+      </c>
+      <c r="G37" s="11">
+        <f t="shared" si="7"/>
+        <v>336.05</v>
+      </c>
+      <c r="H37" s="11">
+        <f t="shared" si="8"/>
+        <v>46.62700000000001</v>
+      </c>
+      <c r="I37" s="8" t="str">
+        <f>I9</f>
+        <v>Mini Control cut out</v>
+      </c>
+      <c r="J37" s="8"/>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="7"/>
+      <c r="C38" s="7"/>
+      <c r="D38" s="7">
+        <v>6</v>
+      </c>
+      <c r="E38" s="7"/>
+      <c r="F38" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G38" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H38" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I38" s="8"/>
+      <c r="J38" s="8"/>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" s="9"/>
+      <c r="B39" s="7"/>
+      <c r="C39" s="7"/>
+      <c r="D39" s="7">
+        <v>5.5</v>
+      </c>
+      <c r="E39" s="7"/>
+      <c r="F39" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G39" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I39" s="8"/>
+      <c r="J39" s="8"/>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="7"/>
+      <c r="C40" s="7"/>
+      <c r="D40" s="7">
+        <v>5</v>
+      </c>
+      <c r="E40" s="7"/>
+      <c r="F40" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G40" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H40" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I40" s="8"/>
+      <c r="J40" s="8"/>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="7"/>
+      <c r="C41" s="7"/>
+      <c r="D41" s="7">
+        <v>4.5</v>
+      </c>
+      <c r="E41" s="7"/>
+      <c r="F41" s="11">
+        <f t="shared" si="6"/>
+        <v>0</v>
+      </c>
+      <c r="G41" s="11">
+        <f t="shared" si="7"/>
+        <v>0</v>
+      </c>
+      <c r="H41" s="11">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="I41" s="8"/>
+      <c r="J41" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="I9:J13"/>
+    <mergeCell ref="A2:A13"/>
+    <mergeCell ref="A16:A27"/>
+    <mergeCell ref="A30:A41"/>
+    <mergeCell ref="I37:J41"/>
+    <mergeCell ref="I23:J27"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>